<commit_message>
Updated translations from Phrase
Updated locale file en-US.xlsx
</commit_message>
<xml_diff>
--- a/en-US.xlsx
+++ b/en-US.xlsx
@@ -26,127 +26,127 @@
     <t>Megerősítés és létrehozás</t>
   </si>
   <si>
-    <t>absence-settings-ui.create-absence-policy-dialog.summary-step</t>
+    <t>absence-settings-ui.create-absence-policy-dialog.summary.annual-entitlement</t>
+  </si>
+  <si>
+    <t>Éves jogosultság</t>
+  </si>
+  <si>
+    <t>absence-settings-ui.create-absence-policy-dialog.summary.annual-entitlement-changes</t>
+  </si>
+  <si>
+    <t>Az alkalmazottak több szabadságot kérhetnek, mint amennyire jogosultak, és ha megadják őket, akkor negatív egyenlegük lesz. Ezt mindig figyelembe veszik a következő ciklus egyenlegének kiszámításakor.</t>
+  </si>
+  <si>
+    <t>absence-settings-ui.create-absence-policy-dialog.summary.annual-entitlement-value</t>
+  </si>
+  <si>
+    <t>:óraszám</t>
+  </si>
+  <si>
+    <t>absence-settings-ui.create-absence-policy-dialog.summary.carryover-label</t>
+  </si>
+  <si>
+    <t>Átvitel</t>
+  </si>
+  <si>
+    <t>absence-settings-ui.create-absence-policy-dialog.summary.carryover.expiry</t>
+  </si>
+  <si>
+    <t>lejár :hónapokkal az időszak vége után</t>
+  </si>
+  <si>
+    <t>absence-settings-ui.create-absence-policy-dialog.summary.carryover.expiry-none</t>
+  </si>
+  <si>
+    <t>nincs lejárat</t>
+  </si>
+  <si>
+    <t>absence-settings-ui.create-absence-policy-dialog.summary.carryover.limit</t>
+  </si>
+  <si>
+    <t>Max. {{hours}}h</t>
+  </si>
+  <si>
+    <t>absence-settings-ui.create-absence-policy-dialog.summary.carryover.not-allowed</t>
+  </si>
+  <si>
+    <t>Nem alllowed</t>
+  </si>
+  <si>
+    <t>absence-settings-ui.create-absence-policy-dialog.summary.granting-cycle-label</t>
+  </si>
+  <si>
+    <t>Engedélyezési ciklus és pillanat</t>
+  </si>
+  <si>
+    <t>absence-settings-ui.create-absence-policy-dialog.summary.granting-cycle.grant-at-end-of-the-month</t>
+  </si>
+  <si>
+    <t>a következő hónap elején</t>
+  </si>
+  <si>
+    <t>absence-settings-ui.create-absence-policy-dialog.summary.granting-cycle.grant-at-start-of-the-month</t>
+  </si>
+  <si>
+    <t>a hónap elején</t>
+  </si>
+  <si>
+    <t>absence-settings-ui.create-absence-policy-dialog.summary.granting-cycle.monthly</t>
+  </si>
+  <si>
+    <t>Havi</t>
+  </si>
+  <si>
+    <t>absence-settings-ui.create-absence-policy-dialog.summary.granting-cycle.yearly</t>
+  </si>
+  <si>
+    <t>Éves</t>
+  </si>
+  <si>
+    <t>absence-settings-ui.create-absence-policy-dialog.summary.policy-name</t>
+  </si>
+  <si>
+    <t>Házirend neve</t>
+  </si>
+  <si>
+    <t>absence-settings-ui.create-absence-policy-dialog.summary.proration-end-of-employment</t>
+  </si>
+  <si>
+    <t>Proráció a foglalkoztatás végén</t>
+  </si>
+  <si>
+    <t>absence-settings-ui.create-absence-policy-dialog.summary.proration-start-of-employment</t>
+  </si>
+  <si>
+    <t>A foglalkoztatás megkezdésekor</t>
+  </si>
+  <si>
+    <t>absence-settings-ui.create-absence-policy-dialog.summary.proration.daily</t>
+  </si>
+  <si>
+    <t>Napi</t>
+  </si>
+  <si>
+    <t>absence-settings-ui.create-absence-policy-dialog.summary.proration.monthly</t>
+  </si>
+  <si>
+    <t>absence-settings-ui.create-absence-policy-dialog.summary.proration.none</t>
+  </si>
+  <si>
+    <t>Nincs</t>
+  </si>
+  <si>
+    <t>absence-settings-ui.create-absence-policy-dialog.test.changes</t>
+  </si>
+  <si>
+    <t>Korlátlan átvitel</t>
+  </si>
+  <si>
+    <t>absence-settings-ui.create-absence-policy-test-changes</t>
   </si>
   <si>
     <t>Összefoglaló</t>
-  </si>
-  <si>
-    <t>absence-settings-ui.create-absence-policy-dialog.summary.annual-entitlement</t>
-  </si>
-  <si>
-    <t>Éves jogosultság</t>
-  </si>
-  <si>
-    <t>absence-settings-ui.create-absence-policy-dialog.summary.annual-entitlement-tooltip</t>
-  </si>
-  <si>
-    <t>Az alkalmazottak több szabadságot kérhetnek, mint amennyire jogosultak, és ha megadják őket, akkor negatív egyenlegük lesz. Ezt mindig figyelembe veszik a következő ciklus egyenlegének kiszámításakor.</t>
-  </si>
-  <si>
-    <t>absence-settings-ui.create-absence-policy-dialog.summary.annual-entitlement-value</t>
-  </si>
-  <si>
-    <t>:óraszám</t>
-  </si>
-  <si>
-    <t>absence-settings-ui.create-absence-policy-dialog.summary.carryover-label</t>
-  </si>
-  <si>
-    <t>Átvitel</t>
-  </si>
-  <si>
-    <t>absence-settings-ui.create-absence-policy-dialog.summary.carryover.expiry</t>
-  </si>
-  <si>
-    <t>lejár :hónapokkal az időszak vége után</t>
-  </si>
-  <si>
-    <t>absence-settings-ui.create-absence-policy-dialog.summary.carryover.expiry-none</t>
-  </si>
-  <si>
-    <t>nincs lejárat</t>
-  </si>
-  <si>
-    <t>absence-settings-ui.create-absence-policy-dialog.summary.carryover.limit</t>
-  </si>
-  <si>
-    <t>Max. {{hours}}h</t>
-  </si>
-  <si>
-    <t>absence-settings-ui.create-absence-policy-dialog.summary.carryover.not-allowed</t>
-  </si>
-  <si>
-    <t>Nem alllowed</t>
-  </si>
-  <si>
-    <t>absence-settings-ui.create-absence-policy-dialog.summary.carryover.unlimited</t>
-  </si>
-  <si>
-    <t>Korlátlan átvitel</t>
-  </si>
-  <si>
-    <t>absence-settings-ui.create-absence-policy-dialog.summary.granting-cycle-label</t>
-  </si>
-  <si>
-    <t>Engedélyezési ciklus és pillanat</t>
-  </si>
-  <si>
-    <t>absence-settings-ui.create-absence-policy-dialog.summary.granting-cycle.grant-at-end-of-the-month</t>
-  </si>
-  <si>
-    <t>a következő hónap elején</t>
-  </si>
-  <si>
-    <t>absence-settings-ui.create-absence-policy-dialog.summary.granting-cycle.grant-at-start-of-the-month</t>
-  </si>
-  <si>
-    <t>a hónap elején</t>
-  </si>
-  <si>
-    <t>absence-settings-ui.create-absence-policy-dialog.summary.granting-cycle.monthly</t>
-  </si>
-  <si>
-    <t>Havi</t>
-  </si>
-  <si>
-    <t>absence-settings-ui.create-absence-policy-dialog.summary.granting-cycle.yearly</t>
-  </si>
-  <si>
-    <t>Éves</t>
-  </si>
-  <si>
-    <t>absence-settings-ui.create-absence-policy-dialog.summary.policy-name</t>
-  </si>
-  <si>
-    <t>Házirend neve</t>
-  </si>
-  <si>
-    <t>absence-settings-ui.create-absence-policy-dialog.summary.proration-end-of-employment</t>
-  </si>
-  <si>
-    <t>Proráció a foglalkoztatás végén</t>
-  </si>
-  <si>
-    <t>absence-settings-ui.create-absence-policy-dialog.summary.proration-start-of-employment</t>
-  </si>
-  <si>
-    <t>A foglalkoztatás megkezdésekor</t>
-  </si>
-  <si>
-    <t>absence-settings-ui.create-absence-policy-dialog.summary.proration.daily</t>
-  </si>
-  <si>
-    <t>Napi</t>
-  </si>
-  <si>
-    <t>absence-settings-ui.create-absence-policy-dialog.summary.proration.monthly</t>
-  </si>
-  <si>
-    <t>absence-settings-ui.create-absence-policy-dialog.summary.proration.none</t>
-  </si>
-  <si>
-    <t>Nincs</t>
   </si>
   <si>
     <t>custom-reports.period-cell-tooltip</t>
@@ -971,25 +971,25 @@
         <v>39</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C20" s="0"/>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>41</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>42</v>
       </c>
       <c r="C21" s="0"/>
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>32</v>
       </c>
       <c r="C22" s="0"/>
     </row>

</xml_diff>